<commit_message>
finish evaluation for polysemi dataset
</commit_message>
<xml_diff>
--- a/output-2/drone-polysemi/adatrans/evaluation_adatrans.xlsx
+++ b/output-2/drone-polysemi/adatrans/evaluation_adatrans.xlsx
@@ -725,107 +725,107 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.885345</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.870149</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.901082</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945813</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.950495</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.679245</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.613636</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.846154</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.987179</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.740385</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.913907</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945205</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.86755</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.770588</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -1121,107 +1121,107 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.856492</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.841791</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.871716</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.936585</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.932039</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.618421</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.580247</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.661972</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.795918</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.847826</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.75</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.913183</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.940397</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.859016</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.757225</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -1253,107 +1253,107 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.861492</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.848576</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.874807</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.92823</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.906542</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.95098</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.604317</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.617647</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.591549</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884211</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.976744</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.807692</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.864198</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.833333</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.916129</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.946667</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.861842</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.761628</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -1517,107 +1517,107 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.885865</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.866864</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.905719</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985222</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.990099</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.980392</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.630872</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.602564</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.661972</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.849741</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921348</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.788462</t>
         </is>
       </c>
       <c r="R9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.847896</t>
         </is>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.740113</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -1781,107 +1781,107 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.885865</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.866864</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.905719</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.687898</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.627907</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.863388</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.759615</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.932432</t>
         </is>
       </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985714</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975309</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.963415</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.859935</t>
         </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.754286</t>
         </is>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -1913,107 +1913,107 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.87738</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.864865</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.890263</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.952381</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.925926</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.980392</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.559441</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.555556</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.56338</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.846154</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.987179</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.740385</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.954248</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.973333</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.935897</t>
         </is>
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.954128</t>
         </is>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.934132</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.872483</t>
         </is>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.783133</t>
         </is>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>
@@ -2441,107 +2441,107 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.901163</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.85048</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.958269</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.908213</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.895238</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.729282</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.929577</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.976077</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.971429</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.980769</t>
         </is>
       </c>
       <c r="R16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921053</t>
         </is>
       </c>
       <c r="S16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.963415</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.940476</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.869565</t>
         </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.778443</t>
         </is>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>
@@ -2705,107 +2705,107 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.86858</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.849335</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.888717</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.926829</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.92233</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.931373</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.633094</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.647059</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.619718</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.938776</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.895899</t>
         </is>
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.904459</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.830189</t>
         </is>
       </c>
       <c r="Y18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.709677</t>
         </is>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -3497,107 +3497,107 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.880419</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.852388</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.910355</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.890995</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.862385</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.642857</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.556701</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.858639</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.942529</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.788462</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.873333</t>
         </is>
       </c>
       <c r="Y24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.779762</t>
         </is>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -4157,107 +4157,107 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.923192</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.891931</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.956723</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.943396</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.909091</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.980392</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.829268</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.731183</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.957746</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.928571</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.98913</t>
         </is>
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.875</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="V29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.877076</t>
         </is>
       </c>
       <c r="Y29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.781065</t>
         </is>
       </c>
       <c r="Z29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
     </row>
@@ -4289,107 +4289,107 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.890869</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.857143</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.927357</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.91866</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897196</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.941176</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.693333</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.658228</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.732394</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.95</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.989583</t>
         </is>
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.913462</t>
         </is>
       </c>
       <c r="R30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.934132</t>
         </is>
       </c>
       <c r="V30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.896552</t>
         </is>
       </c>
       <c r="W30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.859016</t>
         </is>
       </c>
       <c r="Y30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.757225</t>
         </is>
       </c>
       <c r="Z30" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -4685,107 +4685,107 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.87519</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.862069</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.888717</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.933333</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.907407</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.960784</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.613139</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.636364</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.591549</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.855769</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.855769</t>
         </is>
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.855769</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.966887</t>
         </is>
       </c>
       <c r="S33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.935897</t>
         </is>
       </c>
       <c r="U33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.925081</t>
         </is>
       </c>
       <c r="V33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.965986</t>
         </is>
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.870432</t>
         </is>
       </c>
       <c r="Y33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.775148</t>
         </is>
       </c>
       <c r="Z33" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -5345,107 +5345,107 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.891892</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.867153</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.918083</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.94</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.959184</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.710526</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.666667</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.89899</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.946809</t>
         </is>
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.855769</t>
         </is>
       </c>
       <c r="R38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.965944</t>
         </is>
       </c>
       <c r="V38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.957055</t>
         </is>
       </c>
       <c r="W38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.845161</t>
         </is>
       </c>
       <c r="Y38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.735955</t>
         </is>
       </c>
       <c r="Z38" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -6137,107 +6137,107 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.896603</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.858557</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.938176</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.942308</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.924528</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.960784</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.728395</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.648352</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.830986</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.911765</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.93</t>
         </is>
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.894231</t>
         </is>
       </c>
       <c r="R44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.939597</t>
         </is>
       </c>
       <c r="S44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985915</t>
         </is>
       </c>
       <c r="T44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.968944</t>
         </is>
       </c>
       <c r="V44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.962963</t>
         </is>
       </c>
       <c r="W44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.847896</t>
         </is>
       </c>
       <c r="Y44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.740113</t>
         </is>
       </c>
       <c r="Z44" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -6665,107 +6665,107 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.875283</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.856509</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8949</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.980583</t>
         </is>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.971154</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.990196</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.683544</t>
         </is>
       </c>
       <c r="M48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.62069</t>
         </is>
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.875676</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.778846</t>
         </is>
       </c>
       <c r="R48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.925081</t>
         </is>
       </c>
       <c r="V48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.965986</t>
         </is>
       </c>
       <c r="W48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.8875</t>
         </is>
       </c>
       <c r="X48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.821317</t>
         </is>
       </c>
       <c r="Y48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.700535</t>
         </is>
       </c>
       <c r="Z48" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -6797,107 +6797,107 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.888889</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.869822</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.90881</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.937198</t>
         </is>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.92381</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.95098</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.683544</t>
         </is>
       </c>
       <c r="M49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.62069</t>
         </is>
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.760563</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.821053</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.906977</t>
         </is>
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.75</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.945946</t>
         </is>
       </c>
       <c r="S49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.897436</t>
         </is>
       </c>
       <c r="U49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975309</t>
         </is>
       </c>
       <c r="V49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.963415</t>
         </is>
       </c>
       <c r="W49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.9875</t>
         </is>
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.885135</t>
         </is>
       </c>
       <c r="Y49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.79878</t>
         </is>
       </c>
       <c r="Z49" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -6929,107 +6929,107 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.892857</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.860832</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.927357</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.908213</t>
         </is>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.895238</t>
         </is>
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.758621</t>
         </is>
       </c>
       <c r="M50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.640777</t>
         </is>
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.929577</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.865979</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.933333</t>
         </is>
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.807692</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.932432</t>
         </is>
       </c>
       <c r="S50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.985714</t>
         </is>
       </c>
       <c r="T50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="V50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="W50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.975</t>
         </is>
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.870432</t>
         </is>
       </c>
       <c r="Y50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.775148</t>
         </is>
       </c>
       <c r="Z50" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.992424</t>
         </is>
       </c>
     </row>
@@ -7457,107 +7457,107 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.877351</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.854839</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.901082</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.903846</t>
         </is>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.886792</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.921569</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.649007</t>
         </is>
       </c>
       <c r="M54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.6125</t>
         </is>
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.690141</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.88172</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="Q54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.788462</t>
         </is>
       </c>
       <c r="R54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.938776</t>
         </is>
       </c>
       <c r="S54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>1.0</t>
         </is>
       </c>
       <c r="T54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.884615</t>
         </is>
       </c>
       <c r="U54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.963636</t>
         </is>
       </c>
       <c r="V54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.935294</t>
         </is>
       </c>
       <c r="W54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.99375</t>
         </is>
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.846906</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.742857</t>
         </is>
       </c>
       <c r="Z54" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>0.984848</t>
         </is>
       </c>
     </row>

</xml_diff>